<commit_message>
Utilidades Minería de Datos
</commit_message>
<xml_diff>
--- a/corruption_dataset.xlsx
+++ b/corruption_dataset.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="000" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="001" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="002" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm__FilterDatabase" vbProcedure="false">'000'!$A$1:$BL$24</definedName>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="142">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -278,6 +280,177 @@
   </si>
   <si>
     <t xml:space="preserve">UA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Año</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bélgica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulgaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comunidad Helvética</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chipre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alemania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinamarca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">España</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finlandia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Francia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gran Bretaña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hungría</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irlanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Países Bajos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noruega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portugal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rusia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suecia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eslovenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eslovakia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ucrania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abbreviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulgary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czech Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyprus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Britain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hungary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switzerland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovakia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukraine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belgium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kosovo</t>
   </si>
 </sst>
 </file>
@@ -413,11 +586,11 @@
   </sheetPr>
   <dimension ref="A1:BJ24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="61" style="0" width="11.41"/>
   </cols>
@@ -4943,4 +5116,476 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>